<commit_message>
Update schedule + slides
update from 5/6 Session 2
</commit_message>
<xml_diff>
--- a/OneDM-online-conf-schedule-may2020.xlsx
+++ b/OneDM-online-conf-schedule-may2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkoster/Desktop/Conference2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D2144BC-534F-C04A-995C-BF424FA26589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C716BA6-F97F-4E49-9C24-3B7D2A48752C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="16820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,26 +51,26 @@
     <t>16:00 - 18:00 (10-12 PT)</t>
   </si>
   <si>
-    <t>Bus/Tech 1</t>
-  </si>
-  <si>
-    <t>Tech - SDF versions, language features</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kickoff, Agenda Bashing, Mix Topics (Koster) Alt Schemas (Ari), Namespaces </t>
   </si>
   <si>
-    <t>Bus 2 (David Mc.) Public statements, etc.</t>
-  </si>
-  <si>
     <t>Tech - Language features</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Continue Discussion from Wed. + SDF Specification including I/D</t>
+  </si>
+  <si>
+    <t>Business/nontec (David Mc.) Public statements, etc. FAQ and explainers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +88,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,6 +168,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -445,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="133" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,14 +532,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -571,10 +581,10 @@
       <c r="B8" s="9"/>
       <c r="C8" s="8"/>
       <c r="D8" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8" s="8"/>
       <c r="H8" s="7"/>

</xml_diff>

<commit_message>
Update schedule for week 2
</commit_message>
<xml_diff>
--- a/OneDM-online-conf-schedule-may2020.xlsx
+++ b/OneDM-online-conf-schedule-may2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkoster/Library/Containers/com.microsoft.Excel/Data/Desktop/Conference2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DA3378-B173-9D46-B590-4C2E2E969126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8373866-5B64-F94D-97C8-8CCCAF1F1137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="16820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,29 +28,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>One Data Model Spring Conference and Working Sessions</t>
   </si>
   <si>
-    <t>World Time</t>
-  </si>
-  <si>
-    <t>19:00 - 21:00</t>
-  </si>
-  <si>
     <t>IETF oauth</t>
   </si>
   <si>
     <t>Holiday  - cancel regular mtg</t>
   </si>
   <si>
-    <t>13:00 - 15:00 (6-8 PT)</t>
-  </si>
-  <si>
-    <t>16:00 - 18:00 (10-12 PT)</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -64,6 +52,27 @@
   </si>
   <si>
     <t>Session 5 -Business/nontec (David Mc.) Public statements, etc. FAQ and explainers</t>
+  </si>
+  <si>
+    <t>Pacific Time</t>
+  </si>
+  <si>
+    <t>6:00 to 8:00</t>
+  </si>
+  <si>
+    <t>9:00 to 11:00</t>
+  </si>
+  <si>
+    <t>11:00 - 13:00</t>
+  </si>
+  <si>
+    <t>12:00 - 14:00</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Session 6</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +180,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,30 +471,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:R9"/>
+  <dimension ref="A2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="133" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="133" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" customWidth="1"/>
-    <col min="8" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="4.5" customWidth="1"/>
-    <col min="14" max="18" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
+    <col min="9" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="4.5" customWidth="1"/>
+    <col min="15" max="19" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>43955</v>
@@ -493,112 +520,130 @@
       <c r="F5" s="4">
         <v>43959</v>
       </c>
-      <c r="H5" s="4">
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="4">
         <v>43962</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>43963</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>43964</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>43965</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>43966</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>43969</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>43970</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <v>43971</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <v>43972</v>
       </c>
-      <c r="R5" s="4">
+      <c r="S5" s="4">
         <v>43973</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:18" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="13"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="8"/>
       <c r="D8" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="8"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="7"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
     </row>
-    <row r="9" spans="1:18" ht="140" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:19" ht="140" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>